<commit_message>
minor fixes to croz2 mission
</commit_message>
<xml_diff>
--- a/doc/overlap_calculator.xlsx
+++ b/doc/overlap_calculator.xlsx
@@ -321,14 +321,14 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +372,7 @@
       </c>
       <c r="D2" s="6" t="n">
         <f aca="false">(B2-$I$7)/B2</f>
-        <v>0.334748738438933</v>
+        <v>0.265929642415375</v>
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">(C2-I$5*I$6)/C2</f>
@@ -406,7 +406,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">(B3-$I$7)/B3</f>
-        <v>0.5010615538292</v>
+        <v>0.449447231811531</v>
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">(C3-I$5*I$6)/C3</f>
@@ -435,7 +435,7 @@
       </c>
       <c r="D4" s="6" t="n">
         <f aca="false">(B4-$I$7)/B4</f>
-        <v>0.60084924306336</v>
+        <v>0.559557785449224</v>
       </c>
       <c r="E4" s="6" t="n">
         <f aca="false">(C4-I$5*I$6)/C4</f>
@@ -462,7 +462,7 @@
       </c>
       <c r="D5" s="6" t="n">
         <f aca="false">(B5-$I$7)/B5</f>
-        <v>0.667374369219466</v>
+        <v>0.632964821207687</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">(C5-I$5*I$6)/C5</f>
@@ -495,7 +495,7 @@
       </c>
       <c r="D6" s="6" t="n">
         <f aca="false">(B6-$I$7)/B6</f>
-        <v>0.71489231647383</v>
+        <v>0.685398418178019</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">(C6-I$5*I$6)/C6</f>
@@ -526,7 +526,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>14</v>
@@ -670,7 +670,7 @@
       </c>
       <c r="I16" s="5" t="n">
         <f aca="false">H16*I5*I8*60/I7</f>
-        <v>93.1034482758621</v>
+        <v>84.375</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>

</xml_diff>